<commit_message>
updates to func defns
</commit_message>
<xml_diff>
--- a/UpdatedTask1-feature_generation.xlsx
+++ b/UpdatedTask1-feature_generation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\somani4\Documents\GitHub\ECE498_Final_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gowthamkuntumalla/Documents/GitHub/Quant_analysis_stock_market/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A932434-BA6D-436E-880D-070D40D7B2EB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676204FE-B609-2D4D-9239-3E64365CF8B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" activeTab="3" xr2:uid="{6979EBDE-FDCA-4B42-918E-2C70D40B6D11}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" activeTab="1" xr2:uid="{6979EBDE-FDCA-4B42-918E-2C70D40B6D11}"/>
   </bookViews>
   <sheets>
     <sheet name="All Features" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Akhilesh" sheetId="5" r:id="rId4"/>
     <sheet name="Research" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,6 +27,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="307">
   <si>
     <t>ADX/DMS</t>
   </si>
@@ -1248,9 +1251,6 @@
   </si>
   <si>
     <t>Trading indicator, Momentum</t>
-  </si>
-  <si>
-    <t>Similar to Stochastic Oscillator, Day traders use this.</t>
   </si>
   <si>
     <t xml:space="preserve">Similar to RSI but uses standard devs. </t>
@@ -1728,18 +1728,18 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2212,7 +2212,7 @@
       <selection activeCell="A39" sqref="A39:A75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="25.1640625" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5" style="6" customWidth="1"/>
@@ -3176,7 +3176,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B112">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B112">
     <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3187,11 +3187,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AE02222-1276-F842-9642-9CFF961D02CE}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" zoomScale="82" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3:J4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="82" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="21"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="21"/>
   <cols>
     <col min="1" max="1" width="29.83203125" style="42" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" style="37" customWidth="1"/>
@@ -3200,7 +3200,7 @@
     <col min="5" max="16384" width="10.6640625" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="40" customFormat="1" ht="23.5">
+    <row r="1" spans="1:10" s="40" customFormat="1" ht="25">
       <c r="A1" s="39" t="s">
         <v>199</v>
       </c>
@@ -3214,7 +3214,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="42">
+    <row r="2" spans="1:10" ht="44">
       <c r="A2" s="38" t="s">
         <v>1</v>
       </c>
@@ -3245,15 +3245,15 @@
       <c r="C3" s="41" t="s">
         <v>259</v>
       </c>
-      <c r="F3" s="56" t="s">
-        <v>307</v>
-      </c>
-      <c r="G3" s="56"/>
-      <c r="H3" s="56"/>
-      <c r="I3" s="56"/>
-      <c r="J3" s="56"/>
-    </row>
-    <row r="4" spans="1:10" ht="63">
+      <c r="F3" s="60" t="s">
+        <v>306</v>
+      </c>
+      <c r="G3" s="60"/>
+      <c r="H3" s="60"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
+    </row>
+    <row r="4" spans="1:10" ht="66">
       <c r="A4" s="38" t="s">
         <v>13</v>
       </c>
@@ -3263,13 +3263,13 @@
       <c r="C4" s="41" t="s">
         <v>260</v>
       </c>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
-    </row>
-    <row r="5" spans="1:10" ht="42">
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="60"/>
+    </row>
+    <row r="5" spans="1:10" ht="44">
       <c r="A5" s="38" t="s">
         <v>19</v>
       </c>
@@ -3280,7 +3280,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" ht="22">
       <c r="A6" s="38" t="s">
         <v>20</v>
       </c>
@@ -3291,7 +3291,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="63">
+    <row r="7" spans="1:10" ht="66">
       <c r="A7" s="38" t="s">
         <v>21</v>
       </c>
@@ -3305,7 +3305,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="42">
+    <row r="8" spans="1:10" ht="44">
       <c r="A8" s="38" t="s">
         <v>22</v>
       </c>
@@ -3316,7 +3316,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="42">
+    <row r="9" spans="1:10" ht="44">
       <c r="A9" s="38" t="s">
         <v>29</v>
       </c>
@@ -3330,7 +3330,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" ht="22">
       <c r="A10" s="38" t="s">
         <v>30</v>
       </c>
@@ -3344,7 +3344,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="84">
+    <row r="11" spans="1:10" ht="88">
       <c r="A11" s="38" t="s">
         <v>33</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="42">
+    <row r="12" spans="1:10" ht="44">
       <c r="A12" s="38" t="s">
         <v>41</v>
       </c>
@@ -3366,7 +3366,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="48">
+    <row r="13" spans="1:10" ht="52">
       <c r="A13" s="38" t="s">
         <v>42</v>
       </c>
@@ -3380,7 +3380,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="42">
+    <row r="14" spans="1:10" ht="44">
       <c r="A14" s="38" t="s">
         <v>48</v>
       </c>
@@ -3391,7 +3391,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="84">
+    <row r="15" spans="1:10" ht="88">
       <c r="A15" s="38" t="s">
         <v>49</v>
       </c>
@@ -3402,7 +3402,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="42">
+    <row r="16" spans="1:10" ht="44">
       <c r="A16" s="38" t="s">
         <v>50</v>
       </c>
@@ -3413,7 +3413,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="42">
+    <row r="17" spans="1:4" ht="44">
       <c r="A17" s="38" t="s">
         <v>58</v>
       </c>
@@ -3427,7 +3427,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="63">
+    <row r="18" spans="1:4" ht="66">
       <c r="A18" s="38" t="s">
         <v>59</v>
       </c>
@@ -3441,7 +3441,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" ht="22">
       <c r="A19" s="38" t="s">
         <v>60</v>
       </c>
@@ -3452,7 +3452,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="42">
+    <row r="20" spans="1:4" ht="44">
       <c r="A20" s="38" t="s">
         <v>61</v>
       </c>
@@ -3463,7 +3463,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="84">
+    <row r="21" spans="1:4" ht="88">
       <c r="A21" s="38" t="s">
         <v>62</v>
       </c>
@@ -3477,7 +3477,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="42">
+    <row r="22" spans="1:4" ht="44">
       <c r="A22" s="38" t="s">
         <v>71</v>
       </c>
@@ -3485,10 +3485,10 @@
         <v>255</v>
       </c>
       <c r="C22" s="41" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="105">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="110">
       <c r="A23" s="38" t="s">
         <v>72</v>
       </c>
@@ -3499,7 +3499,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" ht="22">
       <c r="A24" s="38" t="s">
         <v>73</v>
       </c>
@@ -3510,7 +3510,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" ht="22">
       <c r="A25" s="38" t="s">
         <v>78</v>
       </c>
@@ -3521,7 +3521,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" ht="22">
       <c r="A26" s="38" t="s">
         <v>79</v>
       </c>
@@ -3532,7 +3532,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" ht="22">
       <c r="A27" s="38" t="s">
         <v>83</v>
       </c>
@@ -3543,32 +3543,32 @@
         <v>290</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="42">
+    <row r="28" spans="1:4" ht="22">
       <c r="A28" s="38" t="s">
         <v>89</v>
       </c>
       <c r="B28" s="37" t="s">
         <v>255</v>
       </c>
-      <c r="C28" s="41" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="C28" s="38" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="22">
       <c r="A29" s="38" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B29" s="37" t="s">
         <v>201</v>
       </c>
       <c r="C29" s="41" t="s">
+        <v>291</v>
+      </c>
+      <c r="D29" s="37" t="s">
         <v>292</v>
       </c>
-      <c r="D29" s="37" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+    </row>
+    <row r="30" spans="1:4" ht="22">
       <c r="A30" s="38" t="s">
         <v>93</v>
       </c>
@@ -3576,10 +3576,10 @@
         <v>255</v>
       </c>
       <c r="C30" s="41" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="42">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="66">
       <c r="A31" s="38" t="s">
         <v>94</v>
       </c>
@@ -3590,7 +3590,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="105">
+    <row r="32" spans="1:4" ht="110">
       <c r="A32" s="38" t="s">
         <v>95</v>
       </c>
@@ -3598,10 +3598,10 @@
         <v>201</v>
       </c>
       <c r="C32" s="41" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="105">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="110">
       <c r="A33" s="38" t="s">
         <v>96</v>
       </c>
@@ -3609,10 +3609,10 @@
         <v>201</v>
       </c>
       <c r="C33" s="41" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="63">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="66">
       <c r="A34" s="38" t="s">
         <v>105</v>
       </c>
@@ -3620,13 +3620,13 @@
         <v>201</v>
       </c>
       <c r="C34" s="41" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D34" s="37" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="22">
       <c r="A35" s="38" t="s">
         <v>106</v>
       </c>
@@ -3634,10 +3634,10 @@
         <v>256</v>
       </c>
       <c r="C35" s="41" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="22">
       <c r="A36" s="38" t="s">
         <v>109</v>
       </c>
@@ -3645,10 +3645,10 @@
         <v>255</v>
       </c>
       <c r="C36" s="41" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="22">
       <c r="A37" s="38" t="s">
         <v>110</v>
       </c>
@@ -3656,10 +3656,10 @@
         <v>255</v>
       </c>
       <c r="C37" s="41" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="105">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="110">
       <c r="A38" s="38" t="s">
         <v>119</v>
       </c>
@@ -3667,7 +3667,7 @@
         <v>256</v>
       </c>
       <c r="C38" s="41" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
   </sheetData>
@@ -3742,16 +3742,16 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="42.6640625" customWidth="1"/>
     <col min="3" max="3" width="29.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" ht="17">
       <c r="A1" s="24" t="s">
         <v>206</v>
       </c>
@@ -3771,7 +3771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="108.5">
+    <row r="2" spans="1:7" ht="119">
       <c r="A2" s="28" t="s">
         <v>0</v>
       </c>
@@ -3783,7 +3783,7 @@
       </c>
       <c r="F2" s="31"/>
     </row>
-    <row r="3" spans="1:7" ht="108.5">
+    <row r="3" spans="1:7" ht="119">
       <c r="A3" s="28" t="s">
         <v>16</v>
       </c>
@@ -3794,7 +3794,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="46.5">
+    <row r="4" spans="1:7" ht="51">
       <c r="A4" s="28" t="s">
         <v>17</v>
       </c>
@@ -3805,7 +3805,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="46.5">
+    <row r="5" spans="1:7" ht="68">
       <c r="A5" s="28" t="s">
         <v>18</v>
       </c>
@@ -3816,7 +3816,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="46.5">
+    <row r="6" spans="1:7" ht="51">
       <c r="A6" s="28" t="s">
         <v>27</v>
       </c>
@@ -3827,7 +3827,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="46.5">
+    <row r="7" spans="1:7" ht="51">
       <c r="A7" s="28" t="s">
         <v>31</v>
       </c>
@@ -3838,7 +3838,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="46.5">
+    <row r="8" spans="1:7" ht="51">
       <c r="A8" s="28" t="s">
         <v>32</v>
       </c>
@@ -3849,7 +3849,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="93">
+    <row r="9" spans="1:7" ht="102">
       <c r="A9" s="28" t="s">
         <v>36</v>
       </c>
@@ -3860,7 +3860,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="46.5">
+    <row r="10" spans="1:7" ht="51">
       <c r="A10" s="28" t="s">
         <v>37</v>
       </c>
@@ -3871,7 +3871,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="31">
+    <row r="11" spans="1:7" ht="34">
       <c r="A11" s="28" t="s">
         <v>38</v>
       </c>
@@ -3882,7 +3882,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="46.5">
+    <row r="12" spans="1:7" ht="51">
       <c r="A12" s="28" t="s">
         <v>39</v>
       </c>
@@ -3893,7 +3893,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="31">
+    <row r="13" spans="1:7" ht="34">
       <c r="A13" s="28" t="s">
         <v>40</v>
       </c>
@@ -3904,7 +3904,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="31">
+    <row r="14" spans="1:7" ht="34">
       <c r="A14" s="28" t="s">
         <v>43</v>
       </c>
@@ -3915,7 +3915,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="62">
+    <row r="15" spans="1:7" ht="68">
       <c r="A15" s="28" t="s">
         <v>51</v>
       </c>
@@ -3926,7 +3926,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="46.5">
+    <row r="16" spans="1:7" ht="51">
       <c r="A16" s="28" t="s">
         <v>52</v>
       </c>
@@ -3937,7 +3937,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="46.5">
+    <row r="17" spans="1:3" ht="51">
       <c r="A17" s="28" t="s">
         <v>63</v>
       </c>
@@ -3948,7 +3948,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="31">
+    <row r="18" spans="1:3" ht="34">
       <c r="A18" s="28" t="s">
         <v>64</v>
       </c>
@@ -3959,7 +3959,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="77.5">
+    <row r="19" spans="1:3" ht="85">
       <c r="A19" s="28" t="s">
         <v>65</v>
       </c>
@@ -3970,7 +3970,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="46.5">
+    <row r="20" spans="1:3" ht="51">
       <c r="A20" s="28" t="s">
         <v>66</v>
       </c>
@@ -3981,7 +3981,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="46.5">
+    <row r="21" spans="1:3" ht="68">
       <c r="A21" s="28" t="s">
         <v>74</v>
       </c>
@@ -3992,7 +3992,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="77.5">
+    <row r="22" spans="1:3" ht="85">
       <c r="A22" s="28" t="s">
         <v>75</v>
       </c>
@@ -4003,7 +4003,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="46.5">
+    <row r="23" spans="1:3" ht="51">
       <c r="A23" s="28" t="s">
         <v>76</v>
       </c>
@@ -4014,7 +4014,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="93">
+    <row r="24" spans="1:3" ht="102">
       <c r="A24" s="28" t="s">
         <v>77</v>
       </c>
@@ -4025,7 +4025,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="31">
+    <row r="25" spans="1:3" ht="34">
       <c r="A25" s="28" t="s">
         <v>84</v>
       </c>
@@ -4036,7 +4036,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="46.5">
+    <row r="26" spans="1:3" ht="51">
       <c r="A26" s="28" t="s">
         <v>86</v>
       </c>
@@ -4047,7 +4047,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="31">
+    <row r="27" spans="1:3" ht="34">
       <c r="A27" s="28" t="s">
         <v>87</v>
       </c>
@@ -4058,7 +4058,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="124">
+    <row r="28" spans="1:3" ht="136">
       <c r="A28" s="28" t="s">
         <v>88</v>
       </c>
@@ -4069,7 +4069,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="46.5">
+    <row r="29" spans="1:3" ht="51">
       <c r="A29" s="28" t="s">
         <v>97</v>
       </c>
@@ -4080,7 +4080,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="77.5">
+    <row r="30" spans="1:3" ht="85">
       <c r="A30" s="28" t="s">
         <v>98</v>
       </c>
@@ -4091,7 +4091,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="93">
+    <row r="31" spans="1:3" ht="102">
       <c r="A31" s="28" t="s">
         <v>99</v>
       </c>
@@ -4102,7 +4102,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="31">
+    <row r="32" spans="1:3" ht="34">
       <c r="A32" s="28" t="s">
         <v>100</v>
       </c>
@@ -4113,7 +4113,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="46.5">
+    <row r="33" spans="1:3" ht="51">
       <c r="A33" s="28" t="s">
         <v>104</v>
       </c>
@@ -4124,7 +4124,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="77.5">
+    <row r="34" spans="1:3" ht="85">
       <c r="A34" s="28" t="s">
         <v>111</v>
       </c>
@@ -4135,7 +4135,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="31">
+    <row r="35" spans="1:3" ht="34">
       <c r="A35" s="28" t="s">
         <v>112</v>
       </c>
@@ -4146,7 +4146,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="31">
+    <row r="36" spans="1:3" ht="34">
       <c r="A36" s="28" t="s">
         <v>113</v>
       </c>
@@ -4157,7 +4157,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="31">
+    <row r="37" spans="1:3" ht="51">
       <c r="A37" s="28" t="s">
         <v>114</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="31">
+    <row r="38" spans="1:3" ht="34">
       <c r="A38" s="28" t="s">
         <v>115</v>
       </c>
@@ -4188,18 +4188,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{364DD11A-90DE-054D-9738-15F07178DAD1}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="25.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.1640625" customWidth="1"/>
     <col min="3" max="3" width="70.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="23" customFormat="1" ht="18.5" thickBot="1">
+    <row r="1" spans="1:6" s="23" customFormat="1" ht="19" thickBot="1">
       <c r="A1" s="45" t="s">
         <v>129</v>
       </c>
@@ -4578,14 +4578,14 @@
         <v>192</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="61" customFormat="1">
-      <c r="A37" s="58" t="s">
+    <row r="37" spans="1:3" s="59" customFormat="1">
+      <c r="A37" s="56" t="s">
         <v>117</v>
       </c>
-      <c r="B37" s="59" t="s">
+      <c r="B37" s="57" t="s">
         <v>195</v>
       </c>
-      <c r="C37" s="60" t="s">
+      <c r="C37" s="58" t="s">
         <v>194</v>
       </c>
     </row>
@@ -4648,17 +4648,17 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="22.5" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.5">
-      <c r="A1" s="57" t="s">
+    <row r="1" spans="1:3" ht="19">
+      <c r="A1" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="57"/>
+      <c r="B1" s="61"/>
       <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:3">
@@ -4687,10 +4687,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="6" spans="1:3">

</xml_diff>

<commit_message>
Automization of all features
</commit_message>
<xml_diff>
--- a/UpdatedTask1-feature_generation.xlsx
+++ b/UpdatedTask1-feature_generation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gowthamkuntumalla/Documents/GitHub/Quant_analysis_stock_market/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\somani4\Documents\GitHub\ECE498_Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{676204FE-B609-2D4D-9239-3E64365CF8B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43563C5C-AEF7-46C7-85A0-2AEF200212A9}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" activeTab="1" xr2:uid="{6979EBDE-FDCA-4B42-918E-2C70D40B6D11}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" activeTab="3" xr2:uid="{6979EBDE-FDCA-4B42-918E-2C70D40B6D11}"/>
   </bookViews>
   <sheets>
     <sheet name="All Features" sheetId="1" r:id="rId1"/>
@@ -1609,7 +1609,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -1634,7 +1634,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1734,12 +1733,14 @@
     <xf numFmtId="0" fontId="26" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="25" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2212,7 +2213,7 @@
       <selection activeCell="A39" sqref="A39:A75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="25.1640625" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5" style="6" customWidth="1"/>
@@ -3176,7 +3177,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B112">
+  <sortState ref="A2:B112">
     <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3187,62 +3188,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AE02222-1276-F842-9642-9CFF961D02CE}">
   <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="82" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="82" workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="21"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="21"/>
   <cols>
-    <col min="1" max="1" width="29.83203125" style="42" customWidth="1"/>
-    <col min="2" max="2" width="24.33203125" style="37" customWidth="1"/>
-    <col min="3" max="3" width="57.6640625" style="41" customWidth="1"/>
-    <col min="4" max="4" width="30.5" style="37" customWidth="1"/>
-    <col min="5" max="16384" width="10.6640625" style="36"/>
+    <col min="1" max="1" width="29.83203125" style="41" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" style="36" customWidth="1"/>
+    <col min="3" max="3" width="57.6640625" style="40" customWidth="1"/>
+    <col min="4" max="4" width="30.5" style="36" customWidth="1"/>
+    <col min="5" max="16384" width="10.6640625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="40" customFormat="1" ht="25">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:10" s="39" customFormat="1" ht="23.5">
+      <c r="A1" s="38" t="s">
         <v>199</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="38" t="s">
         <v>204</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="38" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="44">
-      <c r="A2" s="38" t="s">
+    <row r="2" spans="1:10" ht="42">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="40" t="s">
         <v>258</v>
       </c>
-      <c r="G2" s="35" t="s">
+      <c r="G2" s="34" t="s">
         <v>201</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="34" t="s">
         <v>255</v>
       </c>
-      <c r="I2" s="35" t="s">
+      <c r="I2" s="34" t="s">
         <v>256</v>
       </c>
-      <c r="J2" s="35"/>
+      <c r="J2" s="34"/>
     </row>
     <row r="3" spans="1:10" ht="22" customHeight="1">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="40" t="s">
         <v>259</v>
       </c>
       <c r="F3" s="60" t="s">
@@ -3253,14 +3254,14 @@
       <c r="I3" s="60"/>
       <c r="J3" s="60"/>
     </row>
-    <row r="4" spans="1:10" ht="66">
-      <c r="A4" s="38" t="s">
+    <row r="4" spans="1:10" ht="63">
+      <c r="A4" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="40" t="s">
         <v>260</v>
       </c>
       <c r="F4" s="60"/>
@@ -3269,404 +3270,404 @@
       <c r="I4" s="60"/>
       <c r="J4" s="60"/>
     </row>
-    <row r="5" spans="1:10" ht="44">
-      <c r="A5" s="38" t="s">
+    <row r="5" spans="1:10" ht="42">
+      <c r="A5" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="40" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="22">
-      <c r="A6" s="38" t="s">
+    <row r="6" spans="1:10">
+      <c r="A6" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="40" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="66">
-      <c r="A7" s="38" t="s">
+    <row r="7" spans="1:10" ht="63">
+      <c r="A7" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="36" t="s">
         <v>201</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="40" t="s">
         <v>263</v>
       </c>
-      <c r="D7" s="37" t="s">
+      <c r="D7" s="36" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="44">
-      <c r="A8" s="38" t="s">
+    <row r="8" spans="1:10" ht="42">
+      <c r="A8" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="40" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="44">
-      <c r="A9" s="38" t="s">
+    <row r="9" spans="1:10" ht="42">
+      <c r="A9" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="36" t="s">
         <v>201</v>
       </c>
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="40" t="s">
         <v>268</v>
       </c>
-      <c r="D9" s="43" t="s">
+      <c r="D9" s="42" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="22">
-      <c r="A10" s="38" t="s">
+    <row r="10" spans="1:10">
+      <c r="A10" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="36" t="s">
         <v>201</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="40" t="s">
         <v>267</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="36" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="88">
-      <c r="A11" s="38" t="s">
+    <row r="11" spans="1:10" ht="84">
+      <c r="A11" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="36" t="s">
         <v>256</v>
       </c>
-      <c r="C11" s="41" t="s">
+      <c r="C11" s="40" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="44">
-      <c r="A12" s="38" t="s">
+    <row r="12" spans="1:10" ht="42">
+      <c r="A12" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="40" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="52">
-      <c r="A13" s="38" t="s">
+    <row r="13" spans="1:10" ht="48">
+      <c r="A13" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="C13" s="41" t="s">
+      <c r="C13" s="40" t="s">
         <v>273</v>
       </c>
-      <c r="D13" s="44" t="s">
+      <c r="D13" s="43" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="44">
-      <c r="A14" s="38" t="s">
+    <row r="14" spans="1:10" ht="42">
+      <c r="A14" s="37" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="36" t="s">
         <v>256</v>
       </c>
-      <c r="C14" s="41" t="s">
+      <c r="C14" s="40" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="88">
-      <c r="A15" s="38" t="s">
+    <row r="15" spans="1:10" ht="84">
+      <c r="A15" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="36" t="s">
         <v>256</v>
       </c>
-      <c r="C15" s="41" t="s">
+      <c r="C15" s="40" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="44">
-      <c r="A16" s="38" t="s">
+    <row r="16" spans="1:10" ht="42">
+      <c r="A16" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="C16" s="41" t="s">
+      <c r="C16" s="40" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="44">
-      <c r="A17" s="38" t="s">
+    <row r="17" spans="1:4" ht="42">
+      <c r="A17" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="36" t="s">
         <v>201</v>
       </c>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="40" t="s">
         <v>205</v>
       </c>
-      <c r="D17" s="37" t="s">
+      <c r="D17" s="36" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="66">
-      <c r="A18" s="38" t="s">
+    <row r="18" spans="1:4" ht="63">
+      <c r="A18" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="36" t="s">
         <v>201</v>
       </c>
-      <c r="C18" s="41" t="s">
+      <c r="C18" s="40" t="s">
         <v>279</v>
       </c>
-      <c r="D18" s="37" t="s">
+      <c r="D18" s="36" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="22">
-      <c r="A19" s="38" t="s">
+    <row r="19" spans="1:4">
+      <c r="A19" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="37" t="s">
+      <c r="B19" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="C19" s="41" t="s">
+      <c r="C19" s="40" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="44">
-      <c r="A20" s="38" t="s">
+    <row r="20" spans="1:4" ht="42">
+      <c r="A20" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="B20" s="37" t="s">
+      <c r="B20" s="36" t="s">
         <v>256</v>
       </c>
-      <c r="C20" s="41" t="s">
+      <c r="C20" s="40" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="88">
-      <c r="A21" s="38" t="s">
+    <row r="21" spans="1:4" ht="84">
+      <c r="A21" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="36" t="s">
         <v>201</v>
       </c>
-      <c r="C21" s="41" t="s">
+      <c r="C21" s="40" t="s">
         <v>282</v>
       </c>
-      <c r="D21" s="37" t="s">
+      <c r="D21" s="36" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="44">
-      <c r="A22" s="38" t="s">
+    <row r="22" spans="1:4" ht="42">
+      <c r="A22" s="37" t="s">
         <v>71</v>
       </c>
-      <c r="B22" s="37" t="s">
+      <c r="B22" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="C22" s="41" t="s">
+      <c r="C22" s="40" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="110">
-      <c r="A23" s="38" t="s">
+    <row r="23" spans="1:4" ht="105">
+      <c r="A23" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="B23" s="37" t="s">
+      <c r="B23" s="36" t="s">
         <v>201</v>
       </c>
-      <c r="C23" s="41" t="s">
+      <c r="C23" s="40" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="22">
-      <c r="A24" s="38" t="s">
+    <row r="24" spans="1:4">
+      <c r="A24" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="C24" s="41" t="s">
+      <c r="C24" s="40" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="22">
-      <c r="A25" s="38" t="s">
+    <row r="25" spans="1:4">
+      <c r="A25" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="B25" s="37" t="s">
+      <c r="B25" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="C25" s="41" t="s">
+      <c r="C25" s="40" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="22">
-      <c r="A26" s="38" t="s">
+    <row r="26" spans="1:4">
+      <c r="A26" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="C26" s="41" t="s">
+      <c r="C26" s="40" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="22">
-      <c r="A27" s="38" t="s">
+    <row r="27" spans="1:4">
+      <c r="A27" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="37" t="s">
+      <c r="B27" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="C27" s="41" t="s">
+      <c r="C27" s="40" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="22">
-      <c r="A28" s="38" t="s">
+    <row r="28" spans="1:4">
+      <c r="A28" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="B28" s="37" t="s">
+      <c r="B28" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="C28" s="38" t="s">
+      <c r="C28" s="37" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="22">
-      <c r="A29" s="38" t="s">
+    <row r="29" spans="1:4">
+      <c r="A29" s="37" t="s">
         <v>293</v>
       </c>
-      <c r="B29" s="37" t="s">
+      <c r="B29" s="36" t="s">
         <v>201</v>
       </c>
-      <c r="C29" s="41" t="s">
+      <c r="C29" s="40" t="s">
         <v>291</v>
       </c>
-      <c r="D29" s="37" t="s">
+      <c r="D29" s="36" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="22">
-      <c r="A30" s="38" t="s">
+    <row r="30" spans="1:4">
+      <c r="A30" s="37" t="s">
         <v>93</v>
       </c>
-      <c r="B30" s="37" t="s">
+      <c r="B30" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="C30" s="41" t="s">
+      <c r="C30" s="40" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="66">
-      <c r="A31" s="38" t="s">
+    <row r="31" spans="1:4" ht="42">
+      <c r="A31" s="37" t="s">
         <v>94</v>
       </c>
-      <c r="B31" s="37" t="s">
+      <c r="B31" s="36" t="s">
         <v>201</v>
       </c>
-      <c r="C31" s="41" t="s">
+      <c r="C31" s="40" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="110">
-      <c r="A32" s="38" t="s">
+    <row r="32" spans="1:4" ht="105">
+      <c r="A32" s="37" t="s">
         <v>95</v>
       </c>
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="36" t="s">
         <v>201</v>
       </c>
-      <c r="C32" s="41" t="s">
+      <c r="C32" s="40" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="110">
-      <c r="A33" s="38" t="s">
+    <row r="33" spans="1:4" ht="105">
+      <c r="A33" s="37" t="s">
         <v>96</v>
       </c>
-      <c r="B33" s="37" t="s">
+      <c r="B33" s="36" t="s">
         <v>201</v>
       </c>
-      <c r="C33" s="41" t="s">
+      <c r="C33" s="40" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="66">
-      <c r="A34" s="38" t="s">
+    <row r="34" spans="1:4" ht="63">
+      <c r="A34" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="B34" s="37" t="s">
+      <c r="B34" s="36" t="s">
         <v>201</v>
       </c>
-      <c r="C34" s="41" t="s">
+      <c r="C34" s="40" t="s">
         <v>300</v>
       </c>
-      <c r="D34" s="37" t="s">
+      <c r="D34" s="36" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="22">
-      <c r="A35" s="38" t="s">
+    <row r="35" spans="1:4">
+      <c r="A35" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="B35" s="37" t="s">
+      <c r="B35" s="36" t="s">
         <v>256</v>
       </c>
-      <c r="C35" s="41" t="s">
+      <c r="C35" s="40" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="22">
-      <c r="A36" s="38" t="s">
+    <row r="36" spans="1:4">
+      <c r="A36" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="B36" s="37" t="s">
+      <c r="B36" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="C36" s="41" t="s">
+      <c r="C36" s="40" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="22">
-      <c r="A37" s="38" t="s">
+    <row r="37" spans="1:4">
+      <c r="A37" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="B37" s="37" t="s">
+      <c r="B37" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="C37" s="41" t="s">
+      <c r="C37" s="40" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="110">
-      <c r="A38" s="38" t="s">
+    <row r="38" spans="1:4" ht="105">
+      <c r="A38" s="37" t="s">
         <v>119</v>
       </c>
-      <c r="B38" s="37" t="s">
+      <c r="B38" s="36" t="s">
         <v>256</v>
       </c>
-      <c r="C38" s="41" t="s">
+      <c r="C38" s="40" t="s">
         <v>304</v>
       </c>
     </row>
@@ -3745,437 +3746,437 @@
       <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="2" max="2" width="42.6640625" customWidth="1"/>
     <col min="3" max="3" width="29.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:7">
+      <c r="A1" s="23" t="s">
         <v>206</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>204</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
         <v>207</v>
       </c>
-      <c r="E1" s="25">
+      <c r="E1" s="24">
         <v>5</v>
       </c>
-      <c r="F1" s="26">
+      <c r="F1" s="25">
         <v>3</v>
       </c>
-      <c r="G1" s="27">
+      <c r="G1" s="26">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="119">
-      <c r="A2" s="28" t="s">
+    <row r="2" spans="1:7" ht="108.5">
+      <c r="A2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="28" t="s">
         <v>208</v>
       </c>
-      <c r="C2" s="30" t="s">
+      <c r="C2" s="29" t="s">
         <v>209</v>
       </c>
-      <c r="F2" s="31"/>
-    </row>
-    <row r="3" spans="1:7" ht="119">
-      <c r="A3" s="28" t="s">
+      <c r="F2" s="30"/>
+    </row>
+    <row r="3" spans="1:7" ht="108.5">
+      <c r="A3" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="31" t="s">
         <v>210</v>
       </c>
-      <c r="C3" s="33" t="s">
+      <c r="C3" s="32" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="51">
-      <c r="A4" s="28" t="s">
+    <row r="4" spans="1:7" ht="46.5">
+      <c r="A4" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="29" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="68">
-      <c r="A5" s="28" t="s">
+    <row r="5" spans="1:7" ht="46.5">
+      <c r="A5" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="27" t="s">
         <v>214</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="29" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="51">
-      <c r="A6" s="28" t="s">
+    <row r="6" spans="1:7" ht="46.5">
+      <c r="A6" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="27" t="s">
         <v>215</v>
       </c>
-      <c r="C6" s="34" t="s">
+      <c r="C6" s="33" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="51">
-      <c r="A7" s="28" t="s">
+    <row r="7" spans="1:7" ht="46.5">
+      <c r="A7" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="C7" s="34" t="s">
+      <c r="C7" s="33" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="51">
-      <c r="A8" s="28" t="s">
+    <row r="8" spans="1:7" ht="46.5">
+      <c r="A8" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="27" t="s">
         <v>218</v>
       </c>
-      <c r="C8" s="34" t="s">
+      <c r="C8" s="33" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="102">
-      <c r="A9" s="28" t="s">
+    <row r="9" spans="1:7" ht="93">
+      <c r="A9" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="27" t="s">
         <v>219</v>
       </c>
-      <c r="C9" s="33" t="s">
+      <c r="C9" s="32" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="51">
-      <c r="A10" s="28" t="s">
+    <row r="10" spans="1:7" ht="46.5">
+      <c r="A10" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="27" t="s">
         <v>221</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="29" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="34">
-      <c r="A11" s="28" t="s">
+    <row r="11" spans="1:7" ht="31">
+      <c r="A11" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="27" t="s">
         <v>223</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="29" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="51">
-      <c r="A12" s="28" t="s">
+    <row r="12" spans="1:7" ht="46.5">
+      <c r="A12" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="27" t="s">
         <v>224</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="29" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="34">
-      <c r="A13" s="28" t="s">
+    <row r="13" spans="1:7" ht="31">
+      <c r="A13" s="27" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="27" t="s">
         <v>225</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="29" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="34">
-      <c r="A14" s="28" t="s">
+    <row r="14" spans="1:7" ht="31">
+      <c r="A14" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="27" t="s">
         <v>226</v>
       </c>
-      <c r="C14" s="34" t="s">
+      <c r="C14" s="33" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="68">
-      <c r="A15" s="28" t="s">
+    <row r="15" spans="1:7" ht="62">
+      <c r="A15" s="27" t="s">
         <v>51</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="27" t="s">
         <v>227</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="33" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="51">
-      <c r="A16" s="28" t="s">
+    <row r="16" spans="1:7" ht="46.5">
+      <c r="A16" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="27" t="s">
         <v>228</v>
       </c>
-      <c r="C16" s="33" t="s">
+      <c r="C16" s="32" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="51">
-      <c r="A17" s="28" t="s">
+    <row r="17" spans="1:3" ht="46.5">
+      <c r="A17" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="29" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="34">
-      <c r="A18" s="28" t="s">
+    <row r="18" spans="1:3" ht="31">
+      <c r="A18" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="27" t="s">
         <v>232</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="32" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="85">
-      <c r="A19" s="28" t="s">
+    <row r="19" spans="1:3" ht="77.5">
+      <c r="A19" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="27" t="s">
         <v>233</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="32" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="51">
-      <c r="A20" s="28" t="s">
+    <row r="20" spans="1:3" ht="46.5">
+      <c r="A20" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="27" t="s">
         <v>217</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="C20" s="33" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="68">
-      <c r="A21" s="28" t="s">
+    <row r="21" spans="1:3" ht="46.5">
+      <c r="A21" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="27" t="s">
         <v>235</v>
       </c>
-      <c r="C21" s="34" t="s">
+      <c r="C21" s="33" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="85">
-      <c r="A22" s="28" t="s">
+    <row r="22" spans="1:3" ht="77.5">
+      <c r="A22" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="27" t="s">
         <v>236</v>
       </c>
-      <c r="C22" s="34" t="s">
+      <c r="C22" s="33" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="51">
-      <c r="A23" s="28" t="s">
+    <row r="23" spans="1:3" ht="46.5">
+      <c r="A23" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="27" t="s">
         <v>237</v>
       </c>
-      <c r="C23" s="33" t="s">
+      <c r="C23" s="32" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="102">
-      <c r="A24" s="28" t="s">
+    <row r="24" spans="1:3" ht="93">
+      <c r="A24" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="27" t="s">
         <v>238</v>
       </c>
-      <c r="C24" s="33" t="s">
+      <c r="C24" s="32" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="34">
-      <c r="A25" s="28" t="s">
+    <row r="25" spans="1:3" ht="31">
+      <c r="A25" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="27" t="s">
         <v>239</v>
       </c>
-      <c r="C25" s="34" t="s">
+      <c r="C25" s="33" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="51">
-      <c r="A26" s="28" t="s">
+    <row r="26" spans="1:3" ht="46.5">
+      <c r="A26" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="27" t="s">
         <v>240</v>
       </c>
-      <c r="C26" s="34" t="s">
+      <c r="C26" s="33" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="34">
-      <c r="A27" s="28" t="s">
+    <row r="27" spans="1:3" ht="31">
+      <c r="A27" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="27" t="s">
         <v>240</v>
       </c>
-      <c r="C27" s="34" t="s">
+      <c r="C27" s="33" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="136">
-      <c r="A28" s="28" t="s">
+    <row r="28" spans="1:3" ht="124">
+      <c r="A28" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="27" t="s">
         <v>242</v>
       </c>
-      <c r="C28" s="30" t="s">
+      <c r="C28" s="29" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="51">
-      <c r="A29" s="28" t="s">
+    <row r="29" spans="1:3" ht="46.5">
+      <c r="A29" s="27" t="s">
         <v>97</v>
       </c>
-      <c r="B29" s="28" t="s">
+      <c r="B29" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="C29" s="34" t="s">
+      <c r="C29" s="33" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="85">
-      <c r="A30" s="28" t="s">
+    <row r="30" spans="1:3" ht="77.5">
+      <c r="A30" s="27" t="s">
         <v>98</v>
       </c>
-      <c r="B30" s="28" t="s">
+      <c r="B30" s="27" t="s">
         <v>244</v>
       </c>
-      <c r="C30" s="30" t="s">
+      <c r="C30" s="29" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="102">
-      <c r="A31" s="28" t="s">
+    <row r="31" spans="1:3" ht="93">
+      <c r="A31" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="B31" s="28" t="s">
+      <c r="B31" s="27" t="s">
         <v>246</v>
       </c>
-      <c r="C31" s="34" t="s">
+      <c r="C31" s="33" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="34">
-      <c r="A32" s="28" t="s">
+    <row r="32" spans="1:3" ht="31">
+      <c r="A32" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="B32" s="28" t="s">
+      <c r="B32" s="27" t="s">
         <v>247</v>
       </c>
-      <c r="C32" s="33" t="s">
+      <c r="C32" s="32" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="51">
-      <c r="A33" s="28" t="s">
+    <row r="33" spans="1:3" ht="46.5">
+      <c r="A33" s="27" t="s">
         <v>104</v>
       </c>
-      <c r="B33" s="28" t="s">
+      <c r="B33" s="27" t="s">
         <v>249</v>
       </c>
-      <c r="C33" s="34" t="s">
+      <c r="C33" s="33" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="85">
-      <c r="A34" s="28" t="s">
+    <row r="34" spans="1:3" ht="77.5">
+      <c r="A34" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="B34" s="28" t="s">
+      <c r="B34" s="27" t="s">
         <v>250</v>
       </c>
-      <c r="C34" s="33" t="s">
+      <c r="C34" s="32" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="34">
-      <c r="A35" s="28" t="s">
+    <row r="35" spans="1:3" ht="31">
+      <c r="A35" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="B35" s="28" t="s">
+      <c r="B35" s="27" t="s">
         <v>251</v>
       </c>
-      <c r="C35" s="34" t="s">
+      <c r="C35" s="33" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="34">
-      <c r="A36" s="28" t="s">
+    <row r="36" spans="1:3" ht="31">
+      <c r="A36" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="B36" s="28" t="s">
+      <c r="B36" s="27" t="s">
         <v>252</v>
       </c>
-      <c r="C36" s="34" t="s">
+      <c r="C36" s="33" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="51">
-      <c r="A37" s="28" t="s">
+    <row r="37" spans="1:3" ht="31">
+      <c r="A37" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="B37" s="28" t="s">
+      <c r="B37" s="27" t="s">
         <v>253</v>
       </c>
-      <c r="C37" s="33" t="s">
+      <c r="C37" s="32" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="34">
-      <c r="A38" s="28" t="s">
+    <row r="38" spans="1:3" ht="31">
+      <c r="A38" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="B38" s="28" t="s">
+      <c r="B38" s="27" t="s">
         <v>254</v>
       </c>
-      <c r="C38" s="34" t="s">
+      <c r="C38" s="33" t="s">
         <v>216</v>
       </c>
     </row>
@@ -4188,42 +4189,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{364DD11A-90DE-054D-9738-15F07178DAD1}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="25.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.1640625" customWidth="1"/>
     <col min="3" max="3" width="70.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="23" customFormat="1" ht="19" thickBot="1">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:6" s="22" customFormat="1" ht="18.5" thickBot="1">
+      <c r="A1" s="44" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="46" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="47" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="48" t="s">
         <v>133</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="49" t="s">
         <v>131</v>
       </c>
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
         <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -4234,20 +4235,20 @@
       </c>
       <c r="F3" s="9"/>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="48" t="s">
+    <row r="4" spans="1:6" s="49" customFormat="1">
+      <c r="A4" s="47" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="48" t="s">
         <v>137</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="54" t="s">
         <v>136</v>
       </c>
-      <c r="F4" s="9"/>
+      <c r="F4" s="59"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -4258,7 +4259,7 @@
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>24</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -4269,7 +4270,7 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="19" t="s">
+      <c r="A7" s="18" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -4280,7 +4281,7 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="51" t="s">
+      <c r="A8" s="50" t="s">
         <v>26</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -4291,7 +4292,7 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>28</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -4302,7 +4303,7 @@
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="17" t="s">
         <v>34</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -4312,38 +4313,38 @@
         <v>148</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="18" t="s">
+    <row r="11" spans="1:6" s="49" customFormat="1">
+      <c r="A11" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="62" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:6" s="16" customFormat="1">
-      <c r="A12" s="48" t="s">
+    <row r="12" spans="1:6" s="15" customFormat="1">
+      <c r="A12" s="47" t="s">
         <v>44</v>
       </c>
-      <c r="B12" s="52" t="s">
+      <c r="B12" s="51" t="s">
         <v>152</v>
       </c>
-      <c r="C12" s="53" t="s">
+      <c r="C12" s="52" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="17" t="s">
         <v>45</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="14" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="17" t="s">
         <v>46</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -4354,42 +4355,42 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="17" t="s">
         <v>47</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="14" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="48" t="s">
+      <c r="A16" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="49" t="s">
+      <c r="B16" s="48" t="s">
         <v>159</v>
       </c>
-      <c r="C16" s="54" t="s">
+      <c r="C16" s="53" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="16" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="17" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="17" t="s">
         <v>56</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -4400,7 +4401,7 @@
       </c>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="17" t="s">
         <v>57</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -4411,7 +4412,7 @@
       </c>
     </row>
     <row r="21" spans="1:3">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="17" t="s">
         <v>67</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -4422,23 +4423,23 @@
       </c>
     </row>
     <row r="22" spans="1:3">
-      <c r="A22" s="48" t="s">
+      <c r="A22" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="49" t="s">
+      <c r="B22" s="48" t="s">
         <v>168</v>
       </c>
-      <c r="C22" s="55" t="s">
+      <c r="C22" s="54" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="17" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:3">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="17" t="s">
         <v>70</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -4449,7 +4450,7 @@
       </c>
     </row>
     <row r="25" spans="1:3">
-      <c r="A25" s="48" t="s">
+      <c r="A25" s="17" t="s">
         <v>80</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -4460,40 +4461,40 @@
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="19" t="s">
+      <c r="A26" s="18" t="s">
         <v>81</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="19" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="27" spans="1:3">
-      <c r="A27" s="19" t="s">
+      <c r="A27" s="18" t="s">
         <v>82</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C27" s="21" t="s">
+      <c r="C27" s="20" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="48" t="s">
+    <row r="28" spans="1:3" s="49" customFormat="1">
+      <c r="A28" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="48" t="s">
         <v>178</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="54" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="29" spans="1:3">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="17" t="s">
         <v>91</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -4503,50 +4504,50 @@
         <v>179</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="16" customFormat="1">
-      <c r="A30" s="19" t="s">
+    <row r="30" spans="1:3" s="15" customFormat="1">
+      <c r="A30" s="18" t="s">
         <v>92</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="21" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="16" customFormat="1">
-      <c r="A31" s="18" t="s">
+    <row r="31" spans="1:3" s="15" customFormat="1">
+      <c r="A31" s="17" t="s">
         <v>101</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C31" s="22" t="s">
+      <c r="C31" s="21" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="16" customFormat="1">
-      <c r="A32" s="18" t="s">
+    <row r="32" spans="1:3" s="15" customFormat="1">
+      <c r="A32" s="17" t="s">
         <v>102</v>
       </c>
       <c r="B32"/>
-      <c r="C32" s="22" t="s">
+      <c r="C32" s="21" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="18" t="s">
+    <row r="33" spans="1:3" s="49" customFormat="1">
+      <c r="A33" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="48" t="s">
         <v>187</v>
       </c>
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="54" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="34" spans="1:3">
-      <c r="A34" s="19" t="s">
+      <c r="A34" s="18" t="s">
         <v>107</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -4557,7 +4558,7 @@
       </c>
     </row>
     <row r="35" spans="1:3">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="17" t="s">
         <v>108</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -4568,7 +4569,7 @@
       </c>
     </row>
     <row r="36" spans="1:3">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="18" t="s">
         <v>116</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -4578,25 +4579,25 @@
         <v>192</v>
       </c>
     </row>
-    <row r="37" spans="1:3" s="59" customFormat="1">
-      <c r="A37" s="56" t="s">
+    <row r="37" spans="1:3" s="58" customFormat="1">
+      <c r="A37" s="55" t="s">
         <v>117</v>
       </c>
-      <c r="B37" s="57" t="s">
+      <c r="B37" s="56" t="s">
         <v>195</v>
       </c>
-      <c r="C37" s="58" t="s">
+      <c r="C37" s="57" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="48" t="s">
+    <row r="38" spans="1:3" s="49" customFormat="1">
+      <c r="A38" s="47" t="s">
         <v>118</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="48" t="s">
         <v>198</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="49" t="s">
         <v>196</v>
       </c>
     </row>
@@ -4648,13 +4649,13 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="22.5" customWidth="1"/>
     <col min="2" max="2" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="19">
+    <row r="1" spans="1:3" ht="18.5">
       <c r="A1" s="61" t="s">
         <v>3</v>
       </c>

</xml_diff>